<commit_message>
V0.2.28.6: Strings + Correções
V0.2.28.6: Strings + Correções

+ Adicionados novos espacamentos

+ Adicionado pequenos detalhes aos textos para melhorar sua leitura. (Isso nao tem nem no ingles)

+ Revisado mais de 200k de palavras. Adicionado mais de 100 novas linhas. Corrigido mais de 20 bugs.

+ Arrumado o tamanho de diversos textos sobre os detalhes dos herois.
_____________________________________________

Adicionado: NDN

_____________________________________________

Foi padronizado: N/V (Nada de Novo)

_____________________________________________

Como estou na fase de revisão (ainda terei á de padronização), você vai perceber que a cada atualização, as falas/textos e o jogo parece estar mais fluido, e as conversas estão mais naturais. (Os nomes das Cidades ainda não são permanentes, pois percebi que em algumas partes do jogo, elas não podem ser traduzidas, então provavelmente terei de coloca-las em inglês, após terminar as reviões)
</commit_message>
<xml_diff>
--- a/default-files/Example_ExcelReference/excel/Main/Localization/english/X项目效果_Projects_hotfix.xlsx
+++ b/default-files/Example_ExcelReference/excel/Main/Localization/english/X项目效果_Projects_hotfix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\isyuricunha\Documents\GitHub\sands-of-salzaar-game-translation\default-files\Example_ExcelReference\excel\Main\Localization\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A888722-49F4-4B2F-B70F-A3F905B5F981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A733293-F495-4D68-81F1-3C7EBDD57D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2440,87 +2440,15 @@
     <t>Requisitos não atendidos.</t>
   </si>
   <si>
-    <t>O centro administrativo do acampamento onde são produzidos recursos. Produz 400 Utar, 75 Madeira e 75 Pedra de Ferro toda semana. Adiciona 3 Segurança, 1 Prosperidade e 9 Torres de Turret. Pode-se recrutar 4 equipes de Servos Ifrit a cada semana. Limite de construção: 2.</t>
-  </si>
-  <si>
-    <t>O coração administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Pedra de Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. É possível recrutar uma equipe de Guerreiro Ifrit, Atirador Ifrit, Lançador de Feitiços Ifrit e Cavaleiro Ifrit toda semana. Limite de construção: 3.</t>
-  </si>
-  <si>
-    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 400 Utar, 75 Madeira, 75 Pedra de Ferro e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança, 1 de Prosperidade e 9 Torres de Turret. É possível recrutar 2 equipes de Milícia Nasir e 2 equipes de Infantaria Nasir toda semana. Limite de construção: 2.</t>
-  </si>
-  <si>
-    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Pedra de Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. É possível recrutar uma equipe de Galante Nasir, Lança Longa Nasir, Cavaleiro Nasir, Atirador Nasir e Curandeiro Nasir toda semana. Limite de construção: 3.</t>
-  </si>
-  <si>
-    <t>O coração administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Pedra de Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. É possível recrutar uma equipe de Galante Nasir, Lança Longa Nasir, Cavaleiro Nasir, Atirador Nasir e Curandeiro Nasir toda semana. Limite de construção: 3.</t>
-  </si>
-  <si>
-    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 400 Utar, 75 Madeira e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança, 1 de Prosperidade e 9 Torres de Turret. Pode-se recrutar 1 equipe de Guarda Dhib, 1 equipe de Caçador Dhib e 2 equipes de Pastores Dhib a cada semana. Limite de construção: 2.</t>
-  </si>
-  <si>
-    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Pedra de Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. Pode-se recrutar 1 equipe de Espadachim Dhib, 1 equipe de Lança Longa Dhib e 2 equipes de Rastreadores Dhib a cada semana. Limite de construção: 3.</t>
-  </si>
-  <si>
-    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 700 Utar, 125 Madeira, 125 Pedra de Ferro e 8 Jades toda semana. Adiciona 4 de Segurança, 3 de Prosperidade e 12 Torres de Turret. Pode-se recrutar 2 equipes de Espadachins Dhib, 2 equipes de Lança Longa Dhib e 2 equipes de Rastreadores Dhib a cada semana. Limite de construção: 3.</t>
-  </si>
-  <si>
-    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 400 Utar, 75 Madeira e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança, 1 de Prosperidade e 9 Torres de Turret. É possível recrutar 1 equipe de Espião Dakn e 2 equipes de Lançadores Dakn a cada semana. Limite de construção: 2.</t>
-  </si>
-  <si>
-    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Pedra de Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. É possível recrutar uma equipe de Assassino Dakn, Lançador de Dardos Dakn, Atirador de Espinhos Dakn e Alquimista Dakn toda semana. Limite de construção: 3.</t>
-  </si>
-  <si>
-    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 400 Utar, 75 Madeira, 75 Pedra de Ferro e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança, 1 de Prosperidade e 9 Torres de Turret. É possível recrutar 1 equipe de Guerreiro Thur, 1 equipe de Atirador Thur e 2 equipes de Camponeses Thur a cada semana. Limite de construção: 2.</t>
-  </si>
-  <si>
-    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Pedra de Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. É possível recrutar 1 equipe de Militante Thur, 1 equipe de Arqueiro Exímio Thur e 2 equipes de Infantaria Pesada Thur a cada semana. Limite de construção: 3.</t>
-  </si>
-  <si>
     <t>Atualize para desbloquear mais construções e melhorias, e para recrutar mais tropas.</t>
   </si>
   <si>
-    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança e 9 Torres de Turret. Pode-se recrutar 3 equipes de Milícia Nasir a cada semana. Limite de construção: 1.</t>
-  </si>
-  <si>
-    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança e 12 Torres de Turret. Pode-se recrutar 3 equipes de Milícia Nasir a cada semana. Limite de construção: 1.</t>
-  </si>
-  <si>
-    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança e 9 Torres de Turret. Pode-se recrutar 3 equipes de Moradores Akhal a cada semana. Limite de construção: 1.</t>
-  </si>
-  <si>
-    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança e 12 Torres de Turret. Pode-se recrutar 1 equipe de Cavalaria Leve Akhal e 3 equipes de Moradores Akhal a cada semana. Limite de construção: 1.</t>
-  </si>
-  <si>
-    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança e 9 Torres de Turret. Pode-se recrutar 3 equipes de Pastores Dhib a cada semana. Limite de construção: 1.</t>
-  </si>
-  <si>
-    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira, 75 Pedra de Ferro e 1 Jade toda semana. Adiciona 3 de Segurança e 12 Torres de Turret. Pode-se recrutar 3 equipes de Pastores Dhib a cada semana. Limite de construção: 1.</t>
-  </si>
-  <si>
-    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança e 9 Torres de Turret. Pode-se recrutar 3 equipes de Camponeses Thur a cada semana. Limite de construção: 1.</t>
-  </si>
-  <si>
-    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira, 75 Pedra de Ferro e 1 Jade toda semana. Adiciona 3 de Segurança e 12 Torres de Turret. Pode-se recrutar 3 equipes de Camponeses Thur a cada semana. As equipes guarnecidas aqui recebem 30 EXP por dia. Limite de construção: 1.</t>
-  </si>
-  <si>
-    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança e 9 Torres de Turret. Pode-se recrutar 1 equipe de Lançador Dakn e 2 equipes de Donzelas Dakn a cada semana. Limite de construção: 1.</t>
-  </si>
-  <si>
-    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Pedra de Ferro toda semana. Adiciona 3 de Segurança e 12 Torres de Turret. Pode-se recrutar 1 equipe de Lançador Dakn, 1 equipe de Escorpião Tóxico e 2 equipes de Donzelas Dakn a cada semana. Limite de construção: 1.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Produz 20 unidades de Madeira toda semana. </t>
   </si>
   <si>
     <t xml:space="preserve">Produz 50 unidades de Madeira toda semana. </t>
   </si>
   <si>
-    <t xml:space="preserve">Produz 20 unidades de Pedra de Ferro toda semana. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Produz 50 unidades de Pedra de Ferro toda semana. </t>
-  </si>
-  <si>
     <t>Produz 2 Jades e 1 Prosperidade toda semana. A Prosperidade aumenta o imposto Utar de um assentamento e fornece mais aldeões.</t>
   </si>
   <si>
@@ -2557,9 +2485,6 @@
     <t>Recrute 1 esquadrão de Aprendiz de Mago da Tempestade - Gelo aqui toda semana.</t>
   </si>
   <si>
-    <t>Produz 100 Pedra de Ferro toda semana.</t>
-  </si>
-  <si>
     <t>Recrute 2 esquadrões de Campeões Akhal aqui toda semana.</t>
   </si>
   <si>
@@ -2605,12 +2530,6 @@
     <t>Mais tropas podem ser colocadas em um Acampamento Ifrit. Três esquadrões de tropas podem ser guarnecidos para cada Acampamento Ifrit construído.</t>
   </si>
   <si>
-    <t>O Domínio Ifrit é rico em Jade e Pedra de Ferro. Produz 30 Pedras de Ferro e 3 Jades toda semana.</t>
-  </si>
-  <si>
-    <t>O Domínio Ifrit é rico em Jade e Pedra de Ferro. Produz 50 Pedras de Ferro e 5 Jades toda semana.</t>
-  </si>
-  <si>
     <t>Recrute até 2 Magos Ifrit toda semana.</t>
   </si>
   <si>
@@ -2663,6 +2582,87 @@
   </si>
   <si>
     <t>Construa uma Base</t>
+  </si>
+  <si>
+    <t>O centro administrativo do acampamento onde são produzidos recursos. Produz 400 Utar, 75 Madeira e 75 Ferro toda semana. Adiciona 3 Segurança, 1 Prosperidade e 9 Torres de Turret. Pode-se recrutar 4 equipes de Servos Ifrit a cada semana. Limite de construção: 2.</t>
+  </si>
+  <si>
+    <t>O coração administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. É possível recrutar uma equipe de Guerreiro Ifrit, Atirador Ifrit, Lançador de Feitiços Ifrit e Cavaleiro Ifrit toda semana. Limite de construção: 3.</t>
+  </si>
+  <si>
+    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 400 Utar, 75 Madeira, 75 Ferro e 75 Ferro toda semana. Adiciona 3 de Segurança, 1 de Prosperidade e 9 Torres de Turret. É possível recrutar 2 equipes de Milícia Nasir e 2 equipes de Infantaria Nasir toda semana. Limite de construção: 2.</t>
+  </si>
+  <si>
+    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. É possível recrutar uma equipe de Galante Nasir, Lança Longa Nasir, Cavaleiro Nasir, Atirador Nasir e Curandeiro Nasir toda semana. Limite de construção: 3.</t>
+  </si>
+  <si>
+    <t>O coração administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. É possível recrutar uma equipe de Galante Nasir, Lança Longa Nasir, Cavaleiro Nasir, Atirador Nasir e Curandeiro Nasir toda semana. Limite de construção: 3.</t>
+  </si>
+  <si>
+    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 400 Utar, 75 Madeira e 75 Ferro toda semana. Adiciona 3 de Segurança, 1 de Prosperidade e 9 Torres de Turret. Pode-se recrutar 1 equipe de Guarda Dhib, 1 equipe de Caçador Dhib e 2 equipes de Pastores Dhib a cada semana. Limite de construção: 2.</t>
+  </si>
+  <si>
+    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. Pode-se recrutar 1 equipe de Espadachim Dhib, 1 equipe de Lança Longa Dhib e 2 equipes de Rastreadores Dhib a cada semana. Limite de construção: 3.</t>
+  </si>
+  <si>
+    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 700 Utar, 125 Madeira, 125 Ferro e 8 Jades toda semana. Adiciona 4 de Segurança, 3 de Prosperidade e 12 Torres de Turret. Pode-se recrutar 2 equipes de Espadachins Dhib, 2 equipes de Lança Longa Dhib e 2 equipes de Rastreadores Dhib a cada semana. Limite de construção: 3.</t>
+  </si>
+  <si>
+    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 400 Utar, 75 Madeira e 75 Ferro toda semana. Adiciona 3 de Segurança, 1 de Prosperidade e 9 Torres de Turret. É possível recrutar 1 equipe de Espião Dakn e 2 equipes de Lançadores Dakn a cada semana. Limite de construção: 2.</t>
+  </si>
+  <si>
+    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. É possível recrutar uma equipe de Assassino Dakn, Lançador de Dardos Dakn, Atirador de Espinhos Dakn e Alquimista Dakn toda semana. Limite de construção: 3.</t>
+  </si>
+  <si>
+    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 400 Utar, 75 Madeira, 75 Ferro e 75 Ferro toda semana. Adiciona 3 de Segurança, 1 de Prosperidade e 9 Torres de Turret. É possível recrutar 1 equipe de Guerreiro Thur, 1 equipe de Atirador Thur e 2 equipes de Camponeses Thur a cada semana. Limite de construção: 2.</t>
+  </si>
+  <si>
+    <t>O centro administrativo do acampamento onde os recursos são produzidos. Produz 600 Utar, 100 Madeira, 100 Ferro e 5 Jades toda semana. Adiciona 4 de Segurança, 2 de Prosperidade e 12 Torres de Turret. É possível recrutar 1 equipe de Militante Thur, 1 equipe de Arqueiro Exímio Thur e 2 equipes de Infantaria Pesada Thur a cada semana. Limite de construção: 3.</t>
+  </si>
+  <si>
+    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Ferro toda semana. Adiciona 3 de Segurança e 9 Torres de Turret. Pode-se recrutar 3 equipes de Milícia Nasir a cada semana. Limite de construção: 1.</t>
+  </si>
+  <si>
+    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Ferro toda semana. Adiciona 3 de Segurança e 12 Torres de Turret. Pode-se recrutar 3 equipes de Milícia Nasir a cada semana. Limite de construção: 1.</t>
+  </si>
+  <si>
+    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Ferro toda semana. Adiciona 3 de Segurança e 9 Torres de Turret. Pode-se recrutar 3 equipes de Moradores Akhal a cada semana. Limite de construção: 1.</t>
+  </si>
+  <si>
+    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Ferro toda semana. Adiciona 3 de Segurança e 12 Torres de Turret. Pode-se recrutar 1 equipe de Cavalaria Leve Akhal e 3 equipes de Moradores Akhal a cada semana. Limite de construção: 1.</t>
+  </si>
+  <si>
+    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Ferro toda semana. Adiciona 3 de Segurança e 9 Torres de Turret. Pode-se recrutar 3 equipes de Pastores Dhib a cada semana. Limite de construção: 1.</t>
+  </si>
+  <si>
+    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira, 75 Ferro e 1 Jade toda semana. Adiciona 3 de Segurança e 12 Torres de Turret. Pode-se recrutar 3 equipes de Pastores Dhib a cada semana. Limite de construção: 1.</t>
+  </si>
+  <si>
+    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Ferro toda semana. Adiciona 3 de Segurança e 9 Torres de Turret. Pode-se recrutar 3 equipes de Camponeses Thur a cada semana. Limite de construção: 1.</t>
+  </si>
+  <si>
+    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira, 75 Ferro e 1 Jade toda semana. Adiciona 3 de Segurança e 12 Torres de Turret. Pode-se recrutar 3 equipes de Camponeses Thur a cada semana. As equipes guarnecidas aqui recebem 30 EXP por dia. Limite de construção: 1.</t>
+  </si>
+  <si>
+    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Ferro toda semana. Adiciona 3 de Segurança e 9 Torres de Turret. Pode-se recrutar 1 equipe de Lançador Dakn e 2 equipes de Donzelas Dakn a cada semana. Limite de construção: 1.</t>
+  </si>
+  <si>
+    <t>Um posto avançado com capacidades defensivas limitadas e espaço para tropas guarnecidas. Produz 300 Utar, 75 Madeira e 75 Ferro toda semana. Adiciona 3 de Segurança e 12 Torres de Turret. Pode-se recrutar 1 equipe de Lançador Dakn, 1 equipe de Escorpião Tóxico e 2 equipes de Donzelas Dakn a cada semana. Limite de construção: 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produz 20 unidades de Ferro toda semana. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produz 50 unidades de Ferro toda semana. </t>
+  </si>
+  <si>
+    <t>Produz 100 Ferro toda semana.</t>
+  </si>
+  <si>
+    <t>O Domínio Ifrit é rico em Jade e Ferro. Produz 30 Pedras de Ferro e 3 Jades toda semana.</t>
+  </si>
+  <si>
+    <t>O Domínio Ifrit é rico em Jade e Ferro. Produz 50 Pedras de Ferro e 5 Jades toda semana.</t>
   </si>
 </sst>
 </file>
@@ -3370,8 +3370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G195" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G196" sqref="G196"/>
+    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3419,7 +3419,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="76" t="s">
-        <v>798</v>
+        <v>846</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="276">
@@ -3437,7 +3437,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>799</v>
+        <v>847</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="216">
@@ -3455,7 +3455,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="76" t="s">
-        <v>800</v>
+        <v>848</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="288">
@@ -3473,7 +3473,7 @@
         <v>18</v>
       </c>
       <c r="G5" s="76" t="s">
-        <v>801</v>
+        <v>849</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="216">
@@ -3491,7 +3491,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="76" t="s">
-        <v>800</v>
+        <v>848</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="288">
@@ -3509,7 +3509,7 @@
         <v>18</v>
       </c>
       <c r="G7" s="76" t="s">
-        <v>802</v>
+        <v>850</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="240">
@@ -3527,7 +3527,7 @@
         <v>25</v>
       </c>
       <c r="G8" s="76" t="s">
-        <v>803</v>
+        <v>851</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="264">
@@ -3545,7 +3545,7 @@
         <v>28</v>
       </c>
       <c r="G9" s="76" t="s">
-        <v>804</v>
+        <v>852</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="264">
@@ -3563,7 +3563,7 @@
         <v>31</v>
       </c>
       <c r="G10" s="76" t="s">
-        <v>805</v>
+        <v>853</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="216">
@@ -3581,7 +3581,7 @@
         <v>34</v>
       </c>
       <c r="G11" s="76" t="s">
-        <v>806</v>
+        <v>854</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="276">
@@ -3599,7 +3599,7 @@
         <v>36</v>
       </c>
       <c r="G12" s="76" t="s">
-        <v>807</v>
+        <v>855</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="240">
@@ -3617,7 +3617,7 @@
         <v>38</v>
       </c>
       <c r="G13" s="76" t="s">
-        <v>808</v>
+        <v>856</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="264">
@@ -3635,7 +3635,7 @@
         <v>40</v>
       </c>
       <c r="G14" s="76" t="s">
-        <v>809</v>
+        <v>857</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="72">
@@ -3653,7 +3653,7 @@
         <v>42</v>
       </c>
       <c r="G15" s="76" t="s">
-        <v>810</v>
+        <v>798</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="72">
@@ -3671,7 +3671,7 @@
         <v>42</v>
       </c>
       <c r="G16" s="76" t="s">
-        <v>810</v>
+        <v>798</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="228">
@@ -3689,7 +3689,7 @@
         <v>46</v>
       </c>
       <c r="G17" s="76" t="s">
-        <v>811</v>
+        <v>858</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="240">
@@ -3707,7 +3707,7 @@
         <v>49</v>
       </c>
       <c r="G18" s="76" t="s">
-        <v>812</v>
+        <v>859</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="228">
@@ -3725,7 +3725,7 @@
         <v>51</v>
       </c>
       <c r="G19" s="76" t="s">
-        <v>813</v>
+        <v>860</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="252">
@@ -3743,7 +3743,7 @@
         <v>54</v>
       </c>
       <c r="G20" s="76" t="s">
-        <v>814</v>
+        <v>861</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="228">
@@ -3761,7 +3761,7 @@
         <v>56</v>
       </c>
       <c r="G21" s="76" t="s">
-        <v>815</v>
+        <v>862</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="264">
@@ -3779,7 +3779,7 @@
         <v>59</v>
       </c>
       <c r="G22" s="76" t="s">
-        <v>816</v>
+        <v>863</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="228">
@@ -3797,7 +3797,7 @@
         <v>61</v>
       </c>
       <c r="G23" s="76" t="s">
-        <v>817</v>
+        <v>864</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="300">
@@ -3815,7 +3815,7 @@
         <v>64</v>
       </c>
       <c r="G24" s="76" t="s">
-        <v>818</v>
+        <v>865</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="252">
@@ -3833,7 +3833,7 @@
         <v>66</v>
       </c>
       <c r="G25" s="76" t="s">
-        <v>819</v>
+        <v>866</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="264">
@@ -3851,7 +3851,7 @@
         <v>69</v>
       </c>
       <c r="G26" s="76" t="s">
-        <v>820</v>
+        <v>867</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="48">
@@ -3874,7 +3874,7 @@
         <v>73</v>
       </c>
       <c r="G27" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="120">
@@ -3897,7 +3897,7 @@
         <v>77</v>
       </c>
       <c r="G28" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="48">
@@ -3920,7 +3920,7 @@
         <v>80</v>
       </c>
       <c r="G29" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="108">
@@ -3943,7 +3943,7 @@
         <v>84</v>
       </c>
       <c r="G30" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="144">
@@ -3966,7 +3966,7 @@
         <v>87</v>
       </c>
       <c r="G31" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="144">
@@ -3989,7 +3989,7 @@
         <v>91</v>
       </c>
       <c r="G32" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="120">
@@ -4012,7 +4012,7 @@
         <v>94</v>
       </c>
       <c r="G33" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="120">
@@ -4035,7 +4035,7 @@
         <v>98</v>
       </c>
       <c r="G34" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="72">
@@ -4058,7 +4058,7 @@
         <v>73</v>
       </c>
       <c r="G35" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="144">
@@ -4081,7 +4081,7 @@
         <v>77</v>
       </c>
       <c r="G36" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="72">
@@ -4104,7 +4104,7 @@
         <v>80</v>
       </c>
       <c r="G37" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="144">
@@ -4127,7 +4127,7 @@
         <v>84</v>
       </c>
       <c r="G38" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="144">
@@ -4150,7 +4150,7 @@
         <v>87</v>
       </c>
       <c r="G39" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="144">
@@ -4173,7 +4173,7 @@
         <v>91</v>
       </c>
       <c r="G40" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="120">
@@ -4196,7 +4196,7 @@
         <v>94</v>
       </c>
       <c r="G41" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="144">
@@ -4219,7 +4219,7 @@
         <v>98</v>
       </c>
       <c r="G42" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="72">
@@ -4242,7 +4242,7 @@
         <v>73</v>
       </c>
       <c r="G43" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="144">
@@ -4265,7 +4265,7 @@
         <v>77</v>
       </c>
       <c r="G44" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="72">
@@ -4288,7 +4288,7 @@
         <v>80</v>
       </c>
       <c r="G45" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="144">
@@ -4311,7 +4311,7 @@
         <v>84</v>
       </c>
       <c r="G46" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="144">
@@ -4334,7 +4334,7 @@
         <v>87</v>
       </c>
       <c r="G47" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="144">
@@ -4357,7 +4357,7 @@
         <v>91</v>
       </c>
       <c r="G48" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="120">
@@ -4380,7 +4380,7 @@
         <v>94</v>
       </c>
       <c r="G49" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="144">
@@ -4403,7 +4403,7 @@
         <v>98</v>
       </c>
       <c r="G50" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="84">
@@ -4426,7 +4426,7 @@
         <v>73</v>
       </c>
       <c r="G51" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="156">
@@ -4449,7 +4449,7 @@
         <v>77</v>
       </c>
       <c r="G52" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="84">
@@ -4472,7 +4472,7 @@
         <v>80</v>
       </c>
       <c r="G53" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="144">
@@ -4495,7 +4495,7 @@
         <v>84</v>
       </c>
       <c r="G54" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="144">
@@ -4518,7 +4518,7 @@
         <v>87</v>
       </c>
       <c r="G55" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="156">
@@ -4541,7 +4541,7 @@
         <v>91</v>
       </c>
       <c r="G56" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="120">
@@ -4564,7 +4564,7 @@
         <v>94</v>
       </c>
       <c r="G57" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="144">
@@ -4587,7 +4587,7 @@
         <v>98</v>
       </c>
       <c r="G58" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="84">
@@ -4610,7 +4610,7 @@
         <v>73</v>
       </c>
       <c r="G59" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="156">
@@ -4633,7 +4633,7 @@
         <v>77</v>
       </c>
       <c r="G60" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="84">
@@ -4656,7 +4656,7 @@
         <v>80</v>
       </c>
       <c r="G61" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="156">
@@ -4679,7 +4679,7 @@
         <v>84</v>
       </c>
       <c r="G62" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="144">
@@ -4702,7 +4702,7 @@
         <v>87</v>
       </c>
       <c r="G63" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="156">
@@ -4725,7 +4725,7 @@
         <v>91</v>
       </c>
       <c r="G64" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="120">
@@ -4748,7 +4748,7 @@
         <v>94</v>
       </c>
       <c r="G65" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="156">
@@ -4771,7 +4771,7 @@
         <v>98</v>
       </c>
       <c r="G66" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="84">
@@ -4794,7 +4794,7 @@
         <v>73</v>
       </c>
       <c r="G67" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="144">
@@ -4817,7 +4817,7 @@
         <v>77</v>
       </c>
       <c r="G68" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="84">
@@ -4840,7 +4840,7 @@
         <v>80</v>
       </c>
       <c r="G69" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="144">
@@ -4863,7 +4863,7 @@
         <v>84</v>
       </c>
       <c r="G70" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="144">
@@ -4886,7 +4886,7 @@
         <v>87</v>
       </c>
       <c r="G71" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="144">
@@ -4909,7 +4909,7 @@
         <v>91</v>
       </c>
       <c r="G72" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="120">
@@ -4932,7 +4932,7 @@
         <v>94</v>
       </c>
       <c r="G73" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="144">
@@ -4955,7 +4955,7 @@
         <v>98</v>
       </c>
       <c r="G74" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="84">
@@ -4978,7 +4978,7 @@
         <v>73</v>
       </c>
       <c r="G75" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="144">
@@ -5001,7 +5001,7 @@
         <v>77</v>
       </c>
       <c r="G76" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="84">
@@ -5024,7 +5024,7 @@
         <v>80</v>
       </c>
       <c r="G77" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="144">
@@ -5047,7 +5047,7 @@
         <v>84</v>
       </c>
       <c r="G78" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="144">
@@ -5070,7 +5070,7 @@
         <v>87</v>
       </c>
       <c r="G79" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="144">
@@ -5093,7 +5093,7 @@
         <v>91</v>
       </c>
       <c r="G80" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="120">
@@ -5116,7 +5116,7 @@
         <v>94</v>
       </c>
       <c r="G81" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="144">
@@ -5139,7 +5139,7 @@
         <v>98</v>
       </c>
       <c r="G82" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="72">
@@ -5162,7 +5162,7 @@
         <v>73</v>
       </c>
       <c r="G83" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="180">
@@ -5185,7 +5185,7 @@
         <v>77</v>
       </c>
       <c r="G84" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="180">
@@ -5208,7 +5208,7 @@
         <v>184</v>
       </c>
       <c r="G85" s="76" t="s">
-        <v>840</v>
+        <v>815</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="72">
@@ -5231,7 +5231,7 @@
         <v>80</v>
       </c>
       <c r="G86" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="144">
@@ -5254,7 +5254,7 @@
         <v>84</v>
       </c>
       <c r="G87" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="180">
@@ -5277,7 +5277,7 @@
         <v>191</v>
       </c>
       <c r="G88" s="76" t="s">
-        <v>837</v>
+        <v>870</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="144">
@@ -5300,7 +5300,7 @@
         <v>87</v>
       </c>
       <c r="G89" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="180">
@@ -5323,7 +5323,7 @@
         <v>91</v>
       </c>
       <c r="G90" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="120">
@@ -5346,7 +5346,7 @@
         <v>94</v>
       </c>
       <c r="G91" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="180">
@@ -5369,7 +5369,7 @@
         <v>98</v>
       </c>
       <c r="G92" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="252">
@@ -5392,7 +5392,7 @@
         <v>202</v>
       </c>
       <c r="G93" s="76" t="s">
-        <v>829</v>
+        <v>805</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="108">
@@ -5415,7 +5415,7 @@
         <v>206</v>
       </c>
       <c r="G94" s="76" t="s">
-        <v>830</v>
+        <v>806</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="180">
@@ -5438,7 +5438,7 @@
         <v>210</v>
       </c>
       <c r="G95" s="76" t="s">
-        <v>831</v>
+        <v>807</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="72">
@@ -5461,7 +5461,7 @@
         <v>214</v>
       </c>
       <c r="G96" s="76" t="s">
-        <v>832</v>
+        <v>808</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="72">
@@ -5484,7 +5484,7 @@
         <v>217</v>
       </c>
       <c r="G97" s="76" t="s">
-        <v>864</v>
+        <v>837</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="180">
@@ -5507,7 +5507,7 @@
         <v>221</v>
       </c>
       <c r="G98" s="76" t="s">
-        <v>833</v>
+        <v>809</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="180">
@@ -5530,7 +5530,7 @@
         <v>225</v>
       </c>
       <c r="G99" s="76" t="s">
-        <v>834</v>
+        <v>810</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="216">
@@ -5553,7 +5553,7 @@
         <v>229</v>
       </c>
       <c r="G100" s="76" t="s">
-        <v>835</v>
+        <v>811</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="72">
@@ -5576,7 +5576,7 @@
         <v>73</v>
       </c>
       <c r="G101" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="180">
@@ -5599,7 +5599,7 @@
         <v>77</v>
       </c>
       <c r="G102" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="180">
@@ -5622,7 +5622,7 @@
         <v>184</v>
       </c>
       <c r="G103" s="76" t="s">
-        <v>840</v>
+        <v>815</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="72">
@@ -5645,7 +5645,7 @@
         <v>80</v>
       </c>
       <c r="G104" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="144">
@@ -5668,7 +5668,7 @@
         <v>84</v>
       </c>
       <c r="G105" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="180">
@@ -5691,7 +5691,7 @@
         <v>191</v>
       </c>
       <c r="G106" s="76" t="s">
-        <v>837</v>
+        <v>870</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="144">
@@ -5714,7 +5714,7 @@
         <v>87</v>
       </c>
       <c r="G107" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="180">
@@ -5737,7 +5737,7 @@
         <v>91</v>
       </c>
       <c r="G108" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="120">
@@ -5760,7 +5760,7 @@
         <v>94</v>
       </c>
       <c r="G109" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="180">
@@ -5783,7 +5783,7 @@
         <v>98</v>
       </c>
       <c r="G110" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="252">
@@ -5806,7 +5806,7 @@
         <v>202</v>
       </c>
       <c r="G111" s="76" t="s">
-        <v>829</v>
+        <v>805</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="120">
@@ -5829,7 +5829,7 @@
         <v>206</v>
       </c>
       <c r="G112" s="76" t="s">
-        <v>830</v>
+        <v>806</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="180">
@@ -5852,7 +5852,7 @@
         <v>210</v>
       </c>
       <c r="G113" s="76" t="s">
-        <v>831</v>
+        <v>807</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="72">
@@ -5898,7 +5898,7 @@
         <v>217</v>
       </c>
       <c r="G115" s="76" t="s">
-        <v>864</v>
+        <v>837</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="180">
@@ -5921,7 +5921,7 @@
         <v>221</v>
       </c>
       <c r="G116" s="76" t="s">
-        <v>833</v>
+        <v>809</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="180">
@@ -5944,7 +5944,7 @@
         <v>225</v>
       </c>
       <c r="G117" s="76" t="s">
-        <v>834</v>
+        <v>810</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="216">
@@ -5967,7 +5967,7 @@
         <v>229</v>
       </c>
       <c r="G118" s="76" t="s">
-        <v>835</v>
+        <v>811</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="180">
@@ -6059,7 +6059,7 @@
         <v>73</v>
       </c>
       <c r="G122" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="180">
@@ -6082,7 +6082,7 @@
         <v>77</v>
       </c>
       <c r="G123" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="180">
@@ -6105,7 +6105,7 @@
         <v>184</v>
       </c>
       <c r="G124" s="76" t="s">
-        <v>840</v>
+        <v>815</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="84">
@@ -6128,7 +6128,7 @@
         <v>80</v>
       </c>
       <c r="G125" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="156">
@@ -6151,7 +6151,7 @@
         <v>84</v>
       </c>
       <c r="G126" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="180">
@@ -6174,7 +6174,7 @@
         <v>191</v>
       </c>
       <c r="G127" s="76" t="s">
-        <v>837</v>
+        <v>870</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="144">
@@ -6197,7 +6197,7 @@
         <v>87</v>
       </c>
       <c r="G128" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="180">
@@ -6220,7 +6220,7 @@
         <v>91</v>
       </c>
       <c r="G129" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="120">
@@ -6243,7 +6243,7 @@
         <v>94</v>
       </c>
       <c r="G130" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="180">
@@ -6266,7 +6266,7 @@
         <v>98</v>
       </c>
       <c r="G131" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="252">
@@ -6289,7 +6289,7 @@
         <v>202</v>
       </c>
       <c r="G132" s="76" t="s">
-        <v>829</v>
+        <v>805</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="120">
@@ -6381,7 +6381,7 @@
         <v>217</v>
       </c>
       <c r="G136" s="76" t="s">
-        <v>864</v>
+        <v>837</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="180">
@@ -6404,7 +6404,7 @@
         <v>221</v>
       </c>
       <c r="G137" s="76" t="s">
-        <v>833</v>
+        <v>809</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="180">
@@ -6427,7 +6427,7 @@
         <v>225</v>
       </c>
       <c r="G138" s="76" t="s">
-        <v>834</v>
+        <v>810</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="72">
@@ -6450,7 +6450,7 @@
         <v>73</v>
       </c>
       <c r="G139" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="168">
@@ -6473,7 +6473,7 @@
         <v>77</v>
       </c>
       <c r="G140" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="168">
@@ -6496,7 +6496,7 @@
         <v>184</v>
       </c>
       <c r="G141" s="76" t="s">
-        <v>840</v>
+        <v>815</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="72">
@@ -6519,7 +6519,7 @@
         <v>80</v>
       </c>
       <c r="G142" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="144">
@@ -6542,7 +6542,7 @@
         <v>84</v>
       </c>
       <c r="G143" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="168">
@@ -6565,7 +6565,7 @@
         <v>191</v>
       </c>
       <c r="G144" s="76" t="s">
-        <v>837</v>
+        <v>870</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="144">
@@ -6588,7 +6588,7 @@
         <v>87</v>
       </c>
       <c r="G145" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="168">
@@ -6611,7 +6611,7 @@
         <v>91</v>
       </c>
       <c r="G146" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="120">
@@ -6634,7 +6634,7 @@
         <v>94</v>
       </c>
       <c r="G147" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="168">
@@ -6657,7 +6657,7 @@
         <v>98</v>
       </c>
       <c r="G148" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="252">
@@ -6680,7 +6680,7 @@
         <v>202</v>
       </c>
       <c r="G149" s="76" t="s">
-        <v>829</v>
+        <v>805</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="108">
@@ -6703,7 +6703,7 @@
         <v>206</v>
       </c>
       <c r="G150" s="76" t="s">
-        <v>830</v>
+        <v>806</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="180">
@@ -6726,7 +6726,7 @@
         <v>210</v>
       </c>
       <c r="G151" s="76" t="s">
-        <v>831</v>
+        <v>807</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="72">
@@ -6749,7 +6749,7 @@
         <v>340</v>
       </c>
       <c r="G152" s="76" t="s">
-        <v>836</v>
+        <v>812</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="72">
@@ -6772,7 +6772,7 @@
         <v>217</v>
       </c>
       <c r="G153" s="76" t="s">
-        <v>864</v>
+        <v>837</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="180">
@@ -6795,7 +6795,7 @@
         <v>221</v>
       </c>
       <c r="G154" s="76" t="s">
-        <v>833</v>
+        <v>809</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="180">
@@ -6818,7 +6818,7 @@
         <v>225</v>
       </c>
       <c r="G155" s="76" t="s">
-        <v>834</v>
+        <v>810</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="72">
@@ -6841,7 +6841,7 @@
         <v>73</v>
       </c>
       <c r="G156" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="168">
@@ -6864,7 +6864,7 @@
         <v>77</v>
       </c>
       <c r="G157" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="168">
@@ -6887,7 +6887,7 @@
         <v>184</v>
       </c>
       <c r="G158" s="76" t="s">
-        <v>840</v>
+        <v>815</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="72">
@@ -6910,7 +6910,7 @@
         <v>80</v>
       </c>
       <c r="G159" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="144">
@@ -6933,7 +6933,7 @@
         <v>84</v>
       </c>
       <c r="G160" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="168">
@@ -6956,7 +6956,7 @@
         <v>191</v>
       </c>
       <c r="G161" s="76" t="s">
-        <v>837</v>
+        <v>870</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="144">
@@ -6979,7 +6979,7 @@
         <v>87</v>
       </c>
       <c r="G162" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="168">
@@ -7002,7 +7002,7 @@
         <v>91</v>
       </c>
       <c r="G163" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="164" spans="1:7" ht="120">
@@ -7025,7 +7025,7 @@
         <v>94</v>
       </c>
       <c r="G164" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="168">
@@ -7048,7 +7048,7 @@
         <v>98</v>
       </c>
       <c r="G165" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="252">
@@ -7071,7 +7071,7 @@
         <v>202</v>
       </c>
       <c r="G166" s="76" t="s">
-        <v>829</v>
+        <v>805</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="108">
@@ -7094,7 +7094,7 @@
         <v>206</v>
       </c>
       <c r="G167" s="76" t="s">
-        <v>830</v>
+        <v>806</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="180">
@@ -7117,7 +7117,7 @@
         <v>210</v>
       </c>
       <c r="G168" s="76" t="s">
-        <v>831</v>
+        <v>807</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="72">
@@ -7140,7 +7140,7 @@
         <v>214</v>
       </c>
       <c r="G169" s="76" t="s">
-        <v>832</v>
+        <v>808</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="108">
@@ -7163,7 +7163,7 @@
         <v>374</v>
       </c>
       <c r="G170" s="76" t="s">
-        <v>838</v>
+        <v>813</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="72">
@@ -7186,7 +7186,7 @@
         <v>217</v>
       </c>
       <c r="G171" s="76" t="s">
-        <v>864</v>
+        <v>837</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="180">
@@ -7209,7 +7209,7 @@
         <v>221</v>
       </c>
       <c r="G172" s="76" t="s">
-        <v>833</v>
+        <v>809</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="180">
@@ -7232,7 +7232,7 @@
         <v>225</v>
       </c>
       <c r="G173" s="76" t="s">
-        <v>834</v>
+        <v>810</v>
       </c>
     </row>
     <row r="174" spans="1:7" ht="144">
@@ -7255,7 +7255,7 @@
         <v>383</v>
       </c>
       <c r="G174" s="76" t="s">
-        <v>839</v>
+        <v>814</v>
       </c>
     </row>
     <row r="175" spans="1:7" ht="144">
@@ -7278,7 +7278,7 @@
         <v>383</v>
       </c>
       <c r="G175" s="76" t="s">
-        <v>839</v>
+        <v>814</v>
       </c>
     </row>
     <row r="176" spans="1:7" ht="144">
@@ -7301,7 +7301,7 @@
         <v>383</v>
       </c>
       <c r="G176" s="76" t="s">
-        <v>839</v>
+        <v>814</v>
       </c>
     </row>
     <row r="177" spans="1:7" ht="72">
@@ -7324,7 +7324,7 @@
         <v>73</v>
       </c>
       <c r="G177" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="180">
@@ -7347,7 +7347,7 @@
         <v>77</v>
       </c>
       <c r="G178" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="180">
@@ -7370,7 +7370,7 @@
         <v>184</v>
       </c>
       <c r="G179" s="76" t="s">
-        <v>840</v>
+        <v>815</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="72">
@@ -7393,7 +7393,7 @@
         <v>80</v>
       </c>
       <c r="G180" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="144">
@@ -7416,7 +7416,7 @@
         <v>84</v>
       </c>
       <c r="G181" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="182" spans="1:7" ht="180">
@@ -7439,7 +7439,7 @@
         <v>191</v>
       </c>
       <c r="G182" s="76" t="s">
-        <v>837</v>
+        <v>870</v>
       </c>
     </row>
     <row r="183" spans="1:7" ht="144">
@@ -7462,7 +7462,7 @@
         <v>87</v>
       </c>
       <c r="G183" s="76" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="184" spans="1:7" ht="180">
@@ -7485,7 +7485,7 @@
         <v>91</v>
       </c>
       <c r="G184" s="76" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="185" spans="1:7" ht="120">
@@ -7508,7 +7508,7 @@
         <v>94</v>
       </c>
       <c r="G185" s="76" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
     </row>
     <row r="186" spans="1:7" ht="180">
@@ -7531,7 +7531,7 @@
         <v>98</v>
       </c>
       <c r="G186" s="76" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="252">
@@ -7554,7 +7554,7 @@
         <v>202</v>
       </c>
       <c r="G187" s="76" t="s">
-        <v>829</v>
+        <v>805</v>
       </c>
     </row>
     <row r="188" spans="1:7" ht="108">
@@ -7577,7 +7577,7 @@
         <v>206</v>
       </c>
       <c r="G188" s="76" t="s">
-        <v>830</v>
+        <v>806</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="180">
@@ -7600,7 +7600,7 @@
         <v>210</v>
       </c>
       <c r="G189" s="76" t="s">
-        <v>831</v>
+        <v>807</v>
       </c>
     </row>
     <row r="190" spans="1:7" ht="72">
@@ -7623,7 +7623,7 @@
         <v>416</v>
       </c>
       <c r="G190" s="76" t="s">
-        <v>841</v>
+        <v>816</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="72">
@@ -7646,7 +7646,7 @@
         <v>217</v>
       </c>
       <c r="G191" s="76" t="s">
-        <v>864</v>
+        <v>837</v>
       </c>
     </row>
     <row r="192" spans="1:7" ht="180">
@@ -7669,7 +7669,7 @@
         <v>221</v>
       </c>
       <c r="G192" s="76" t="s">
-        <v>833</v>
+        <v>809</v>
       </c>
     </row>
     <row r="193" spans="1:7" ht="180">
@@ -7692,7 +7692,7 @@
         <v>225</v>
       </c>
       <c r="G193" s="76" t="s">
-        <v>834</v>
+        <v>810</v>
       </c>
     </row>
     <row r="194" spans="1:7" ht="120">
@@ -7715,7 +7715,7 @@
         <v>423</v>
       </c>
       <c r="G194" s="76" t="s">
-        <v>842</v>
+        <v>817</v>
       </c>
     </row>
     <row r="195" spans="1:7" ht="132">
@@ -7738,7 +7738,7 @@
         <v>426</v>
       </c>
       <c r="G195" s="76" t="s">
-        <v>843</v>
+        <v>818</v>
       </c>
     </row>
     <row r="196" spans="1:7" ht="156">
@@ -7761,7 +7761,7 @@
         <v>429</v>
       </c>
       <c r="G196" s="76" t="s">
-        <v>844</v>
+        <v>819</v>
       </c>
     </row>
     <row r="197" spans="1:7" ht="36">
@@ -7784,7 +7784,7 @@
         <v>433</v>
       </c>
       <c r="G197" s="76" t="s">
-        <v>845</v>
+        <v>820</v>
       </c>
     </row>
     <row r="198" spans="1:7" ht="72">
@@ -7807,7 +7807,7 @@
         <v>437</v>
       </c>
       <c r="G198" s="76" t="s">
-        <v>846</v>
+        <v>821</v>
       </c>
     </row>
     <row r="199" spans="1:7" ht="72">
@@ -7830,7 +7830,7 @@
         <v>440</v>
       </c>
       <c r="G199" s="76" t="s">
-        <v>847</v>
+        <v>822</v>
       </c>
     </row>
     <row r="200" spans="1:7" ht="72">
@@ -7853,7 +7853,7 @@
         <v>444</v>
       </c>
       <c r="G200" s="76" t="s">
-        <v>848</v>
+        <v>823</v>
       </c>
     </row>
     <row r="201" spans="1:7" ht="72">
@@ -7876,7 +7876,7 @@
         <v>448</v>
       </c>
       <c r="G201" s="76" t="s">
-        <v>849</v>
+        <v>824</v>
       </c>
     </row>
     <row r="202" spans="1:7" ht="72">
@@ -7899,7 +7899,7 @@
         <v>451</v>
       </c>
       <c r="G202" s="76" t="s">
-        <v>850</v>
+        <v>825</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="72">
@@ -7922,7 +7922,7 @@
         <v>437</v>
       </c>
       <c r="G203" s="76" t="s">
-        <v>846</v>
+        <v>821</v>
       </c>
     </row>
     <row r="204" spans="1:7" ht="72">
@@ -7945,7 +7945,7 @@
         <v>440</v>
       </c>
       <c r="G204" s="76" t="s">
-        <v>847</v>
+        <v>822</v>
       </c>
     </row>
     <row r="205" spans="1:7" ht="72">
@@ -7968,7 +7968,7 @@
         <v>444</v>
       </c>
       <c r="G205" s="76" t="s">
-        <v>848</v>
+        <v>823</v>
       </c>
     </row>
     <row r="206" spans="1:7" ht="72">
@@ -7991,7 +7991,7 @@
         <v>448</v>
       </c>
       <c r="G206" s="76" t="s">
-        <v>849</v>
+        <v>824</v>
       </c>
     </row>
     <row r="207" spans="1:7" ht="72">
@@ -8014,7 +8014,7 @@
         <v>451</v>
       </c>
       <c r="G207" s="76" t="s">
-        <v>850</v>
+        <v>825</v>
       </c>
     </row>
     <row r="208" spans="1:7" ht="96">
@@ -8037,7 +8037,7 @@
         <v>463</v>
       </c>
       <c r="G208" s="76" t="s">
-        <v>851</v>
+        <v>826</v>
       </c>
     </row>
     <row r="209" spans="1:7" ht="108">
@@ -8060,7 +8060,7 @@
         <v>465</v>
       </c>
       <c r="G209" s="76" t="s">
-        <v>852</v>
+        <v>827</v>
       </c>
     </row>
     <row r="210" spans="1:7" ht="120">
@@ -8083,7 +8083,7 @@
         <v>467</v>
       </c>
       <c r="G210" s="76" t="s">
-        <v>853</v>
+        <v>871</v>
       </c>
     </row>
     <row r="211" spans="1:7" ht="120">
@@ -8106,7 +8106,7 @@
         <v>469</v>
       </c>
       <c r="G211" s="76" t="s">
-        <v>854</v>
+        <v>872</v>
       </c>
     </row>
     <row r="212" spans="1:7" ht="48">
@@ -8129,7 +8129,7 @@
         <v>471</v>
       </c>
       <c r="G212" s="76" t="s">
-        <v>855</v>
+        <v>828</v>
       </c>
     </row>
     <row r="213" spans="1:7" ht="60">
@@ -8152,7 +8152,7 @@
         <v>473</v>
       </c>
       <c r="G213" s="76" t="s">
-        <v>856</v>
+        <v>829</v>
       </c>
     </row>
     <row r="214" spans="1:7" ht="48">
@@ -8175,7 +8175,7 @@
         <v>475</v>
       </c>
       <c r="G214" s="76" t="s">
-        <v>857</v>
+        <v>830</v>
       </c>
     </row>
     <row r="215" spans="1:7" ht="36">
@@ -8198,7 +8198,7 @@
         <v>73</v>
       </c>
       <c r="G215" s="76" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
     </row>
     <row r="216" spans="1:7" ht="144">
@@ -8221,7 +8221,7 @@
         <v>77</v>
       </c>
       <c r="G216" s="76" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
     </row>
     <row r="217" spans="1:7" ht="144">
@@ -8244,7 +8244,7 @@
         <v>184</v>
       </c>
       <c r="G217" s="76" t="s">
-        <v>840</v>
+        <v>815</v>
       </c>
     </row>
     <row r="218" spans="1:7" ht="36">
@@ -8267,7 +8267,7 @@
         <v>80</v>
       </c>
       <c r="G218" s="76" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
     </row>
     <row r="219" spans="1:7" ht="108">
@@ -8290,7 +8290,7 @@
         <v>84</v>
       </c>
       <c r="G219" s="76" t="s">
-        <v>824</v>
+        <v>869</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="144">
@@ -8313,7 +8313,7 @@
         <v>191</v>
       </c>
       <c r="G220" s="76" t="s">
-        <v>837</v>
+        <v>870</v>
       </c>
     </row>
     <row r="221" spans="1:7" ht="36">
@@ -8382,7 +8382,7 @@
         <v>487</v>
       </c>
       <c r="G223" s="76" t="s">
-        <v>858</v>
+        <v>831</v>
       </c>
     </row>
     <row r="224" spans="1:7" ht="144">
@@ -8405,7 +8405,7 @@
         <v>490</v>
       </c>
       <c r="G224" s="76" t="s">
-        <v>859</v>
+        <v>832</v>
       </c>
     </row>
     <row r="225" spans="1:7" ht="144">
@@ -8428,7 +8428,7 @@
         <v>492</v>
       </c>
       <c r="G225" s="76" t="s">
-        <v>860</v>
+        <v>833</v>
       </c>
     </row>
     <row r="226" spans="1:7" ht="84">
@@ -8451,7 +8451,7 @@
         <v>494</v>
       </c>
       <c r="G226" s="76" t="s">
-        <v>861</v>
+        <v>834</v>
       </c>
     </row>
     <row r="227" spans="1:7" ht="144">
@@ -8474,7 +8474,7 @@
         <v>497</v>
       </c>
       <c r="G227" s="76" t="s">
-        <v>862</v>
+        <v>835</v>
       </c>
     </row>
     <row r="228" spans="1:7" ht="96">
@@ -8497,7 +8497,7 @@
         <v>500</v>
       </c>
       <c r="G228" s="76" t="s">
-        <v>863</v>
+        <v>836</v>
       </c>
     </row>
     <row r="229" spans="1:7" ht="48">
@@ -8520,7 +8520,7 @@
         <v>217</v>
       </c>
       <c r="G229" s="76" t="s">
-        <v>864</v>
+        <v>837</v>
       </c>
     </row>
     <row r="230" spans="1:7" ht="84">
@@ -8543,7 +8543,7 @@
         <v>502</v>
       </c>
       <c r="G230" s="76" t="s">
-        <v>865</v>
+        <v>838</v>
       </c>
     </row>
     <row r="231" spans="1:7" ht="84">
@@ -8566,7 +8566,7 @@
         <v>504</v>
       </c>
       <c r="G231" s="76" t="s">
-        <v>866</v>
+        <v>839</v>
       </c>
     </row>
     <row r="232" spans="1:7" ht="36">
@@ -8589,7 +8589,7 @@
         <v>506</v>
       </c>
       <c r="G232" s="76" t="s">
-        <v>867</v>
+        <v>840</v>
       </c>
     </row>
     <row r="233" spans="1:7" ht="48">
@@ -8612,7 +8612,7 @@
         <v>508</v>
       </c>
       <c r="G233" s="76" t="s">
-        <v>868</v>
+        <v>841</v>
       </c>
     </row>
     <row r="234" spans="1:7" ht="24">
@@ -8635,7 +8635,7 @@
         <v>510</v>
       </c>
       <c r="G234" s="76" t="s">
-        <v>869</v>
+        <v>842</v>
       </c>
     </row>
     <row r="235" spans="1:7" ht="24">
@@ -8658,7 +8658,7 @@
         <v>512</v>
       </c>
       <c r="G235" s="76" t="s">
-        <v>870</v>
+        <v>843</v>
       </c>
     </row>
     <row r="236" spans="1:7" ht="24">
@@ -8681,7 +8681,7 @@
         <v>512</v>
       </c>
       <c r="G236" s="76" t="s">
-        <v>870</v>
+        <v>843</v>
       </c>
     </row>
     <row r="237" spans="1:7" ht="24">
@@ -8704,7 +8704,7 @@
         <v>512</v>
       </c>
       <c r="G237" s="76" t="s">
-        <v>870</v>
+        <v>843</v>
       </c>
     </row>
     <row r="238" spans="1:7" ht="24">
@@ -8727,7 +8727,7 @@
         <v>516</v>
       </c>
       <c r="G238" s="76" t="s">
-        <v>872</v>
+        <v>845</v>
       </c>
     </row>
     <row r="239" spans="1:7" ht="24">
@@ -8750,7 +8750,7 @@
         <v>518</v>
       </c>
       <c r="G239" s="76" t="s">
-        <v>871</v>
+        <v>844</v>
       </c>
     </row>
     <row r="240" spans="1:7" ht="24">

</xml_diff>